<commit_message>
Informe de avance de pruebas y reporte Sonar Qube
</commit_message>
<xml_diff>
--- a/1. Plan calidad.xlsx
+++ b/1. Plan calidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10. SOFKAU\2. Programación\3. QA\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D16D4E-DA1C-4748-A6FB-7CF73F959C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5D78E2-E888-4211-A1AC-D436F2970005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,6 +49,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t xml:space="preserve">Area </t>
   </si>
@@ -113,49 +114,15 @@
     <t>Externo</t>
   </si>
   <si>
-    <t>Estudiante de Sofka U</t>
-  </si>
-  <si>
     <t>Release</t>
   </si>
   <si>
-    <t>1. Se parte del supuesto que la funcionalidad del flujo de compras de un producto se encuentre estable.</t>
-  </si>
-  <si>
-    <t>se recomiendas pruebas de seguridad
-se recomienda pruebas de rendimiento</t>
-  </si>
-  <si>
-    <t>Las actividades comprometidas durante el alcance se realizaran en los siguientes sprint: Sprint 1: Funcionalidad de todos los campos del carrito de compras al comprar un tipo de producto. Sprint 2: Funcionalidad de todos los campos del carrito de compras al comprar diferentes tipos de productos.</t>
-  </si>
-  <si>
     <t>Verificación de servicio SOA calculadora</t>
   </si>
   <si>
     <t>Se realizarán pruebas funcionales para verificar  la correcta operatividad de la operaciones que incluye la calculadora.</t>
   </si>
   <si>
-    <t>Verificación de servicio SOA convertir numeros a moneda o texto.</t>
-  </si>
-  <si>
-    <t>Verificar que la operación suma efectúa la suma de dos números enteros, verificar que la operación resta efectua la resta entre dos números enteros, verificar que la operación multiplicación efectua la multiplicación de dos números enteros, verificar que la operación división efectua la división de sos números enteros, verificar que no es posible dividir a un numero entero entre cero, verificar que las operaciones suma, resta, multiplicación y división se efectuan bajo constantes como A y B.</t>
-  </si>
-  <si>
-    <t>Verificar que la calculadora opera sumas con más de dos sumandos. Verificar que la calculadora opera multiplicaciónes con más de dos números. Verificar que la calculadora opera con operaciones combinadas.</t>
-  </si>
-  <si>
-    <t>Se realizarán pruebas funcionales para verificar  la conversión de numeros a moneda tipo dólar  y numero en texto.</t>
-  </si>
-  <si>
-    <t>Verificar  la conversión de numero a texto, verificar la conversión de un numero a moneda tipo dólar.</t>
-  </si>
-  <si>
-    <t>Se probará las peticiones SOAT del servicio por medio de pruebas funcionales, donde se verificará la respuesta la operatividad de dos numeros con las operaciones suma, resta, multiplicaciones  y divisiones.</t>
-  </si>
-  <si>
-    <t>Se probará las peticiones SOAT del servicio por medio de pruebas funcionales, donde se verificará la conversión de un valor numerico a moneda tipo  dólar y a valor numerico en texto.</t>
-  </si>
-  <si>
     <t>Q-Gates</t>
   </si>
   <si>
@@ -210,27 +177,93 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>Se realizarán pruebas funcionales para verificar el flujo de compras por parte de un usario que se encuentra registrado en supermercado carulla.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No se realizarán pruebas de rendimiento, no funcionales, automatizadas. </t>
-  </si>
-  <si>
-    <t>Verificar la compra de un producto. -Verificar la compra de multiples productos.  - Verificar metodo de envío.  -Verificar el button eliminar producto del carrito de compra. - Verificar button continuar comprando, - Verificar button editar carrito, -Verificar forma de pago por Bono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se probará el flujo de compra efectuado por un usuario registrado en la plataforma carrulla </t>
-  </si>
-  <si>
-    <t>1. El usuario debe tener acceso a la página web.                                                                                                                                                                                                                                                                                2. El usuario debe estar registrado y con una sesión inciada dentro del portal web de carrulla.
-3. El catálogo de productos debe estár disponible.</t>
+    <t>Las actividades comprometidas durante el alcance se realizarán en las siguientes fases:
+Fase 1: Planificación y diseño del plan de calidad, matriz de riesgos y casos de prueba.
+Fase 2: Ejecución de casos de prueba para el servicio  el servicio de calculadora.</t>
+  </si>
+  <si>
+    <t>Las actividades comprometidas durante el alcance se realizarán en las siguientes fases:
+Fase 1: Planificación y diseño del plan de calidad, matriz de riesgos y casos de prueba.
+Fase 2: Ejecución de casos de prueba para el servicio  el servicio de conversión de unidades.</t>
+  </si>
+  <si>
+    <t>Verificar  la conversión de numero a texto, verificar la conversión de un numero a moneda tipo dólar. Se probará con diferentes tipos de números.</t>
+  </si>
+  <si>
+    <t>No se realizarán pruebas de rendimiento, no funcionales, automatizadas, de integración</t>
+  </si>
+  <si>
+    <t>Se recomiendas pruebas de seguridad
+Se recomienda pruebas de rendimiento                                                                                                                                                                                                                                                                                                se recomienda pruebas de integración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se recomiendas pruebas de seguridad
+Se recomienda pruebas de rendimiento                                                                                                                                                                                                                                                                                                </t>
+  </si>
+  <si>
+    <t>Se asegura la precisión de los resultados generados en las operaciones.</t>
+  </si>
+  <si>
+    <t>Se asegura la precisión en las conversiones realizadas en el servicio.</t>
+  </si>
+  <si>
+    <t>Se realizarán pruebas funcionales para verificar el flujo de compras por parte de un usuario que se encuentra registrado en supermercado Carulla.</t>
+  </si>
+  <si>
+    <t>Verificar la compra de un producto. -Verificar la compra de múltiples productos.  - Verificar el servicio compra y recoge  -Verificar el botón eliminar producto del carrito de compra -Verificar forma de pago por pse, tarjetas de crédito, tuya y cupón. -Verificar la compra de producto por descuento</t>
+  </si>
+  <si>
+    <t>Verificar que la operación suma efectúa la suma de dos números enteros, verificar que la operación resta efectúa la resta entre dos números enteros, verificar que la operación multiplicación efectúa la multiplicación de dos números enteros, verificar que la operación división efectúa la división de los números enteros, verificar que no es posible dividir a un número entero entre cero, verificar que las operaciones suma, resta, multiplicación y división se efectúan bajo constantes como A y B.</t>
+  </si>
+  <si>
+    <t>pruebas de seguridad, pruebas de rendimiento, pruebas de integración, pruebas de carga.</t>
+  </si>
+  <si>
+    <t>Se realizarán pruebas funcionales para verificar la conversión de números a moneda tipo dólar y numero en texto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pruebas de seguridad, pruebas de rendimiento, pruebas de integración, pruebas de carga.
+Verificar que la calculadora opera suma con más de dos sumandos. Verificar que la calculadora opera multiplicaciones con más de dos números. Verificar que la calculadora opera con operaciones combinadas. </t>
+  </si>
+  <si>
+    <t>1. El usuario debe tener acceso a la página web: https://www.carulla.com/.                                                                                                                                                                                                                                                                                2. El usuario debe estar registrado y con una sesión iniciada dentro del portal web de carrulla.
+3. El catálogo de productos debe estar disponible.</t>
+  </si>
+  <si>
+    <t>Se parte del supuesto que la funcionalidad del flujo de compras de un producto se encuentre estable.</t>
+  </si>
+  <si>
+    <t>1. Se debe tener acceso al servicio SOAP: http://www.dneonline.com/calculator.asmx?wsdl                                                                                                                                                                                                       2. Contar la herramienta de prueba SoapUI para probar el servicio web en SOAP.</t>
+  </si>
+  <si>
+    <t>Se probará mediante pruebas manuales el servicio de calculadora,  donde se verificará la respuesta la operatividad de dos números con las operaciones suma, resta, multiplicaciones  y divisiones.</t>
+  </si>
+  <si>
+    <t>Se probará mediante pruebas manuales el sericio de conversión, donde se verificará la conversión de un valor numérico a moneda tipo dólar y a valor numérico en texto.</t>
+  </si>
+  <si>
+    <t>Yolima Alejandra Guadir Paguay</t>
+  </si>
+  <si>
+    <t>Las actividades comprometidas durante el alcance se realizarán en las siguientes fases:
+Fase 1: Planificación y diseño del plan de calidad, matriz de riesgos y casos de prueba.
+Fase 2: Ejecución de casos de prueba para el flujo de carrito de compras en la página web de Carulla</t>
+  </si>
+  <si>
+    <t>Mediante pruebas manuales se probará el flujo de compra efectuado por un usuario registrado en la plataforma carulla, el cual incluye se probar que se agregue los productos al carrito de manera correcta, probar que los métodos de pago sean válidos y modificar la cantidad de productos asignados al carrito de compras.</t>
+  </si>
+  <si>
+    <t>1. Se debe tener acceso al servicio SOAP: https://www.dataaccess.com/webservicesserver/numberconversion.wso?WSDL.                                                                                                                         2. Contar la herramienta de prueba SoapUI para probar el servicio web en SOAP.</t>
+  </si>
+  <si>
+    <t>Verificación de servicio SOAP convertir numeros a moneda o texto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,34 +294,33 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -343,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -629,67 +661,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -707,7 +775,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -716,13 +784,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -736,12 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1461,11 +1523,11 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
@@ -1481,156 +1543,183 @@
     <col min="13" max="13" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+    <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" s="36" customFormat="1" ht="51" customHeight="1">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="114.75">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="14" customFormat="1" ht="229.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="C4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="229.5">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="76.5">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
+      <c r="I5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1651,193 +1740,193 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="33.42578125" style="8" customWidth="1"/>
+    <col min="2" max="5" width="33.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:5">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="35"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="38"/>
+      <c r="C5" s="6">
         <v>30</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="26"/>
-    </row>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="27"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="29"/>
-      <c r="C5" s="10">
-        <v>30</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="7">
         <f>D5/C5</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>34</v>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="29"/>
-      <c r="C7" s="10">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="38"/>
+      <c r="C7" s="6">
         <v>30</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="6">
         <v>7</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="7">
         <f>D7/C7</f>
         <v>0.23333333333333334</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="13" t="s">
-        <v>34</v>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="29"/>
-      <c r="C9" s="32">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="38"/>
+      <c r="C9" s="41">
         <v>20</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="14">
+      <c r="D9" s="40"/>
+      <c r="E9" s="10">
         <f>C9</f>
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30">
-      <c r="B10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>34</v>
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="29"/>
-      <c r="C11" s="10">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="38"/>
+      <c r="C11" s="6">
         <v>1</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="10">
         <f>C11+D11</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>34</v>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="29"/>
-      <c r="C13" s="10">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="38"/>
+      <c r="C13" s="6">
         <v>5</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <v>7</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="7">
         <f>D13/C13</f>
         <v>1.4</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="12" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="39" t="s">
         <v>34</v>
       </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="15" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B15" s="18"/>
-      <c r="C15" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="15" t="str">
+    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="27"/>
+      <c r="C15" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="11" t="str">
         <f>C15</f>
         <v>SI</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B17" s="18"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="27"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>